<commit_message>
Update PTBR localization Excel files
Multiple PTBR language Excel files for dialog and game data have been updated. Changes likely include new or revised translations and content for various game elements.
</commit_message>
<xml_diff>
--- a/PTBR-COM-PORTRAIT/Lang/PTBR/Dialog/Drama/elder_exile.xlsx
+++ b/PTBR-COM-PORTRAIT/Lang/PTBR/Dialog/Drama/elder_exile.xlsx
@@ -1,34 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\PTBR\Lang\PTBR\Dialog\Drama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ysi\Documents\GitHub\elin-portugues-brasileiro\PTBR\Lang\PTBR\Dialog\Drama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC3BEECD-EBED-45BD-8D04-09D449C77464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507AD8FC-5F62-476C-B3A1-C15B7CCBCF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6810" yWindow="1350" windowWidth="21600" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raphael" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr xmlns:loext="http://schemas.libreoffice.org/" stringRefSyntax="CalcA1"/>
     </ext>
@@ -764,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L8" sqref="L8"/>
       <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>

</xml_diff>